<commit_message>
update diccionario variables no usadas
</commit_message>
<xml_diff>
--- a/data/dictionaries/Diccionario.xlsx
+++ b/data/dictionaries/Diccionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DISCOELENA\Proyectos\PythonAnalytics\data\dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811FC9C6-FBA6-46EA-96DE-A657A2A22490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9380B4ED-5DC0-4F61-BF10-D05ADA864C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3E056A65-5D47-4FFF-810A-5E13F76002B2}"/>
   </bookViews>
@@ -271,9 +271,6 @@
     <t>Puntos de cobre</t>
   </si>
   <si>
-    <t>Puntos totales de cobre en la tasa</t>
-  </si>
-  <si>
     <t>Defectos de categoría uno</t>
   </si>
   <si>
@@ -293,6 +290,9 @@
   </si>
   <si>
     <t>Number ICO</t>
+  </si>
+  <si>
+    <t>Puntos totales de la tasa</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +334,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,13 +362,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF67D813-D714-427D-BE17-6EF98F392C94}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +750,7 @@
         <v>70</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +772,7 @@
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,125 +908,127 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="D21" s="8"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
+      <c r="B30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,8 +1049,8 @@
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" t="s">
-        <v>79</v>
+      <c r="C32" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1061,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1083,7 @@
         <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1094,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,28 +1105,28 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>